<commit_message>
Actualización del sitio Quarto
</commit_message>
<xml_diff>
--- a/data/bases_datos.xlsx
+++ b/data/bases_datos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manue\Desktop\lab-econometria\datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manue\Desktop\lab-econometria\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{002E25F3-1DED-491F-819F-2FEAC56487FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91079D64-E31B-4EAC-AE99-512842A3097E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="14400" windowHeight="8145" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="11805" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="encuestas" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="416">
   <si>
     <t>Años</t>
   </si>
@@ -1212,6 +1212,63 @@
   </si>
   <si>
     <t>Permite analizar la evolución de precios y la inflación mediante modelos de series de tiempo, identificando tendencias y factores que afectan el costo de vida.</t>
+  </si>
+  <si>
+    <t>Business Environment and Enterprise Performance Survey (BEEPS) – EBRD &amp; World Bank</t>
+  </si>
+  <si>
+    <t>https://www.ebrd.com/home/what-we-do/office-of-the-chief-economist/beeps/business-environment-enterprise-performance-survey-data.html</t>
+  </si>
+  <si>
+    <t>Encuesta de Desarrollo e Innovación Tecnológica (EDIT) – DANE (Colombia)</t>
+  </si>
+  <si>
+    <t>https://www.dane.gov.co/index.php/estadisticas-por-tema/tecnologia-e-innovacion/encuesta-de-desarrollo-e-innovacion-tecnologica-edit</t>
+  </si>
+  <si>
+    <t>Encuesta Nacional de Innovación – PRODUCE (Perú)</t>
+  </si>
+  <si>
+    <t>https://ogeiee.produce.gob.pe/index.php/en/shortcode/normatividad-metodologia-oee/encuesta-nacional-de-innovacion</t>
+  </si>
+  <si>
+    <t>Encuesta Nacional de Actividades de Ciencia, Tecnología e Innovación (ACTI) – Ecuador</t>
+  </si>
+  <si>
+    <t>https://www.ecuadorencifras.gob.ec/encuesta-nacional-de-actividades-de-ciencia-tecnologia-e-innovacion-acti/</t>
+  </si>
+  <si>
+    <t>EBDR</t>
+  </si>
+  <si>
+    <t>1999-2025</t>
+  </si>
+  <si>
+    <t>EXCEL/CSV/STATA</t>
+  </si>
+  <si>
+    <t>Levanta información estandarizada sobre el entorno de negocios, desempeño de las empresas, obstáculos a la inversión, finanzas, innovación, infraestructura y gobernanza. Está diseñada para comparar países y medir la evolución del clima empresarial, siendo una de las principales fuentes internacionales para estudios de productividad e innovación en economías en transición y mercados emergentes</t>
+  </si>
+  <si>
+    <t>DANE</t>
+  </si>
+  <si>
+    <t>Recoge datos detallados sobre actividades de innovación, inversión en tecnología, adopción digital, barreras, resultados innovadores y vínculos con universidades y centros tecnológicos. Se ajusta a los lineamientos del Manual de Oslo, permitiendo comparaciones internacionales y análisis de capacidades tecnológicas en el sector productivo colombiano.</t>
+  </si>
+  <si>
+    <t>PRODUCE</t>
+  </si>
+  <si>
+    <t>Mide las actividades de innovación, capacidades tecnológicas, inversión en I+D, impactos productivos y desafíos que enfrentan las empresas. Su metodología sigue estándares OCDE, proporcionando datos fundamentales para evaluar la competitividad del sector empresarial peruano, así como la adopción tecnológica y el desempeño innovador por sectores y tamaños de firma</t>
+  </si>
+  <si>
+    <t>INCEC</t>
+  </si>
+  <si>
+    <t>2012-2014</t>
+  </si>
+  <si>
+    <t>Constituye la principal fuente para analizar el ecosistema de ciencia, tecnología e innovación en Ecuador, proporcionando series comparables con estándares internacionales y utilizadas para diagnósticos nacionales y estudios académicos.</t>
   </si>
 </sst>
 </file>
@@ -1589,10 +1646,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2203,6 +2260,86 @@
         <v>396</v>
       </c>
     </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>406</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C31" t="s">
+        <v>397</v>
+      </c>
+      <c r="D31" t="s">
+        <v>398</v>
+      </c>
+      <c r="E31" t="s">
+        <v>407</v>
+      </c>
+      <c r="F31" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>126</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="C32" t="s">
+        <v>399</v>
+      </c>
+      <c r="D32" t="s">
+        <v>400</v>
+      </c>
+      <c r="E32" t="s">
+        <v>407</v>
+      </c>
+      <c r="F32" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>369</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="C33" t="s">
+        <v>401</v>
+      </c>
+      <c r="D33" t="s">
+        <v>402</v>
+      </c>
+      <c r="E33" t="s">
+        <v>407</v>
+      </c>
+      <c r="F33" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>414</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="C34" t="s">
+        <v>403</v>
+      </c>
+      <c r="D34" t="s">
+        <v>404</v>
+      </c>
+      <c r="E34" t="s">
+        <v>59</v>
+      </c>
+      <c r="F34" t="s">
+        <v>415</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2213,7 +2350,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+    <sheetView topLeftCell="A61" workbookViewId="0">
       <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>

</xml_diff>